<commit_message>
adding additional spreadsheets with results and for results analysis
</commit_message>
<xml_diff>
--- a/data/correlation_analysis_intepretation.xlsx
+++ b/data/correlation_analysis_intepretation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ojcchar/repositories/Projects/complexity-verification-project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65CB03F6-D90D-4B41-8B67-1E9818D53527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{803D3A30-CCB4-0D43-B7AC-1B70B661F739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17680" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all_tools" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="55">
   <si>
     <t>metric</t>
   </si>
@@ -206,13 +206,16 @@
   <si>
     <t>% of expected cor (Medium)</t>
   </si>
+  <si>
+    <t>9_nc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -347,7 +350,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -418,9 +421,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,8 +771,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O2" sqref="O2:O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -858,7 +867,7 @@
       <c r="H2" s="5">
         <v>23</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="39">
         <v>-0.33772774774302539</v>
       </c>
       <c r="J2" s="5">
@@ -871,7 +880,7 @@
         <v>6.0216356265286271E-2</v>
       </c>
       <c r="M2" s="22" t="str">
-        <f>IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
         <v>y</v>
       </c>
       <c r="N2" s="23" t="str">
@@ -879,8 +888,8 @@
         <v>Medium</v>
       </c>
       <c r="O2" s="23" t="str">
-        <f>IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" ref="O2:O21" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.01,"**",IF(J2&lt;0.05,"*", "")))</f>
+        <v>*</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -908,7 +917,7 @@
       <c r="H3" s="5">
         <v>23</v>
       </c>
-      <c r="I3" s="5">
+      <c r="I3" s="39">
         <v>-0.42754829069287381</v>
       </c>
       <c r="J3" s="5">
@@ -921,7 +930,7 @@
         <v>7.124393687845218E-3</v>
       </c>
       <c r="M3" s="22" t="str">
-        <f>IF(ISBLANK(I3),"",IF(AND(D3="negative",I3&lt;0),"y",IF(AND(D3="positive",I3&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N3" s="23" t="str">
@@ -929,8 +938,8 @@
         <v>Medium</v>
       </c>
       <c r="O3" s="23" t="str">
-        <f>IF(ISBLANK(I3),"",IF(J3&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="1"/>
+        <v>**</v>
       </c>
     </row>
     <row r="4" spans="1:19" s="5" customFormat="1" x14ac:dyDescent="0.2">
@@ -958,7 +967,7 @@
       <c r="H4" s="5">
         <v>23</v>
       </c>
-      <c r="I4" s="5">
+      <c r="I4" s="39">
         <v>0.41117066001056379</v>
       </c>
       <c r="J4" s="5">
@@ -971,7 +980,7 @@
         <v>8.3820912440796345E-3</v>
       </c>
       <c r="M4" s="22" t="str">
-        <f>IF(ISBLANK(I4),"",IF(AND(D4="negative",I4&lt;0),"y",IF(AND(D4="positive",I4&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N4" s="23" t="str">
@@ -979,8 +988,8 @@
         <v>Medium</v>
       </c>
       <c r="O4" s="23" t="str">
-        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.01,"**",IF(J4&lt;0.05,"*", "")))</f>
+        <v>**</v>
       </c>
     </row>
     <row r="5" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1008,7 +1017,7 @@
       <c r="H5" s="7">
         <v>12</v>
       </c>
-      <c r="I5" s="7">
+      <c r="I5" s="40">
         <v>-0.31333978072025609</v>
       </c>
       <c r="J5" s="7">
@@ -1021,7 +1030,7 @@
         <v>0.31406107950112661</v>
       </c>
       <c r="M5" s="24" t="str">
-        <f>IF(ISBLANK(I5),"",IF(AND(D5="negative",I5&lt;0),"y",IF(AND(D5="positive",I5&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N5" s="25" t="str">
@@ -1029,8 +1038,8 @@
         <v>Medium</v>
       </c>
       <c r="O5" s="25" t="str">
-        <f>IF(ISBLANK(I5),"",IF(J5&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" ref="O5:O21" si="2">IF(ISBLANK(I5),"",IF(J5&lt;0.01,"**",IF(J5&lt;0.05,"*", "")))</f>
+        <v/>
       </c>
     </row>
     <row r="6" spans="1:19" s="7" customFormat="1" x14ac:dyDescent="0.2">
@@ -1058,7 +1067,7 @@
       <c r="H6" s="7">
         <v>12</v>
       </c>
-      <c r="I6" s="7">
+      <c r="I6" s="40">
         <v>-0.45260190548481433</v>
       </c>
       <c r="J6" s="7">
@@ -1071,7 +1080,7 @@
         <v>0.12370498159100569</v>
       </c>
       <c r="M6" s="24" t="str">
-        <f>IF(ISBLANK(I6),"",IF(AND(D6="negative",I6&lt;0),"y",IF(AND(D6="positive",I6&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N6" s="25" t="str">
@@ -1079,8 +1088,8 @@
         <v>Medium</v>
       </c>
       <c r="O6" s="25" t="str">
-        <f>IF(ISBLANK(I6),"",IF(J6&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q6" s="34" t="s">
         <v>44</v>
@@ -1117,7 +1126,7 @@
       <c r="H7" s="7">
         <v>12</v>
       </c>
-      <c r="I7" s="7">
+      <c r="I7" s="40">
         <v>-0.38297084310253521</v>
       </c>
       <c r="J7" s="7">
@@ -1130,7 +1139,7 @@
         <v>0.13405987835546679</v>
       </c>
       <c r="M7" s="24" t="str">
-        <f>IF(ISBLANK(I7),"",IF(AND(D7="negative",I7&lt;0),"y",IF(AND(D7="positive",I7&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N7" s="25" t="str">
@@ -1138,8 +1147,8 @@
         <v>Medium</v>
       </c>
       <c r="O7" s="25" t="str">
-        <f>IF(ISBLANK(I7),"",IF(J7&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q7" s="35">
         <v>0</v>
@@ -1176,7 +1185,7 @@
       <c r="H8" s="7">
         <v>12</v>
       </c>
-      <c r="I8" s="7">
+      <c r="I8" s="40">
         <v>0.13926212476455829</v>
       </c>
       <c r="J8" s="7">
@@ -1189,7 +1198,7 @@
         <v>0.52633237245257225</v>
       </c>
       <c r="M8" s="24" t="str">
-        <f>IF(ISBLANK(I8),"",IF(AND(D8="negative",I8&lt;0),"y",IF(AND(D8="positive",I8&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N8" s="25" t="str">
@@ -1197,8 +1206,8 @@
         <v>Small</v>
       </c>
       <c r="O8" s="25" t="str">
-        <f>IF(ISBLANK(I8),"",IF(J8&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q8" s="35">
         <v>0.1</v>
@@ -1227,28 +1236,28 @@
         <v>100</v>
       </c>
       <c r="F9" s="11">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G9" s="11">
-        <v>392</v>
+        <v>434</v>
       </c>
       <c r="H9" s="11">
         <v>100</v>
       </c>
-      <c r="I9" s="11">
-        <v>-0.22964462414024381</v>
+      <c r="I9" s="41">
+        <v>-0.19033631802488879</v>
       </c>
       <c r="J9" s="11">
-        <v>1.3810859520988481E-3</v>
+        <v>7.5752215667813554E-3</v>
       </c>
       <c r="K9" s="11">
-        <v>-0.32505085088761609</v>
+        <v>-0.27758322655087048</v>
       </c>
       <c r="L9" s="11">
-        <v>9.6778635956533269E-4</v>
+        <v>5.1722673233929881E-3</v>
       </c>
       <c r="M9" s="26" t="str">
-        <f>IF(ISBLANK(I9),"",IF(AND(D9="negative",I9&lt;0),"y",IF(AND(D9="positive",I9&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N9" s="27" t="str">
@@ -1256,8 +1265,8 @@
         <v>Small</v>
       </c>
       <c r="O9" s="27" t="str">
-        <f>IF(ISBLANK(I9),"",IF(J9&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v>**</v>
       </c>
       <c r="Q9" s="36">
         <v>0.3</v>
@@ -1286,28 +1295,28 @@
         <v>50</v>
       </c>
       <c r="F10" s="14">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G10" s="14">
-        <v>156</v>
+        <v>794</v>
       </c>
       <c r="H10" s="14">
         <v>50</v>
       </c>
-      <c r="I10" s="14">
-        <v>-2.1865071526333869E-2</v>
+      <c r="I10" s="42">
+        <v>-1.3914136425848831E-2</v>
       </c>
       <c r="J10" s="14">
-        <v>0.85746045357848777</v>
+        <v>0.90900323668647842</v>
       </c>
       <c r="K10" s="14">
-        <v>-2.3705418235251699E-2</v>
+        <v>-1.0266126007392471E-2</v>
       </c>
       <c r="L10" s="14">
-        <v>0.87019890091340346</v>
+        <v>0.94359018578297449</v>
       </c>
       <c r="M10" s="28" t="str">
-        <f>IF(ISBLANK(I10),"",IF(AND(D10="negative",I10&lt;0),"y",IF(AND(D10="positive",I10&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N10" s="29" t="str">
@@ -1315,8 +1324,8 @@
         <v>None</v>
       </c>
       <c r="O10" s="29" t="str">
-        <f>IF(ISBLANK(I10),"",IF(J10&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q10" s="37">
         <v>0.5</v>
@@ -1345,28 +1354,28 @@
         <v>50</v>
       </c>
       <c r="F11" s="14">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G11" s="14">
-        <v>156</v>
+        <v>794</v>
       </c>
       <c r="H11" s="14">
         <v>50</v>
       </c>
-      <c r="I11" s="14">
+      <c r="I11" s="42">
         <v>-2.8152946873129591E-2</v>
       </c>
       <c r="J11" s="14">
         <v>0.80868009561069343</v>
       </c>
       <c r="K11" s="14">
-        <v>-2.915890758270907E-2</v>
+        <v>-2.99893827986723E-2</v>
       </c>
       <c r="L11" s="14">
-        <v>0.84068897194493819</v>
+        <v>0.83621302723678093</v>
       </c>
       <c r="M11" s="28" t="str">
-        <f>IF(ISBLANK(I11),"",IF(AND(D11="negative",I11&lt;0),"y",IF(AND(D11="positive",I11&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N11" s="29" t="str">
@@ -1374,8 +1383,8 @@
         <v>None</v>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF(ISBLANK(I11),"",IF(J11&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -1395,28 +1404,28 @@
         <v>50</v>
       </c>
       <c r="F12" s="14">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="G12" s="14">
-        <v>156</v>
+        <v>794</v>
       </c>
       <c r="H12" s="14">
         <v>50</v>
       </c>
-      <c r="I12" s="14">
+      <c r="I12" s="42">
         <v>-0.24788466776030799</v>
       </c>
       <c r="J12" s="14">
         <v>3.1887928946905821E-2</v>
       </c>
       <c r="K12" s="14">
-        <v>-0.31090970189222938</v>
+        <v>-0.30961847204159432</v>
       </c>
       <c r="L12" s="14">
-        <v>2.7974705548467111E-2</v>
+        <v>2.8666961474283319E-2</v>
       </c>
       <c r="M12" s="28" t="str">
-        <f>IF(ISBLANK(I12),"",IF(AND(D12="negative",I12&lt;0),"y",IF(AND(D12="positive",I12&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N12" s="29" t="str">
@@ -1424,16 +1433,16 @@
         <v>Small</v>
       </c>
       <c r="O12" s="29" t="str">
-        <f>IF(ISBLANK(I12),"",IF(J12&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="18">
-        <v>9</v>
+      <c r="B13" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>30</v>
@@ -1442,31 +1451,31 @@
         <v>34</v>
       </c>
       <c r="E13" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G13" s="17">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="H13" s="17">
-        <v>30</v>
-      </c>
-      <c r="I13" s="17">
-        <v>-0.35467801654479708</v>
+        <v>10</v>
+      </c>
+      <c r="I13" s="43">
+        <v>-0.45353942022497418</v>
       </c>
       <c r="J13" s="17">
-        <v>1.2621596666894941E-2</v>
+        <v>8.0702142650775008E-2</v>
       </c>
       <c r="K13" s="17">
-        <v>-0.44637709632263278</v>
+        <v>-0.60076029057829006</v>
       </c>
       <c r="L13" s="17">
-        <v>1.341282859891604E-2</v>
+        <v>6.6252950743798139E-2</v>
       </c>
       <c r="M13" s="30" t="str">
-        <f>IF(ISBLANK(I13),"",IF(AND(D13="negative",I13&lt;0),"y",IF(AND(D13="positive",I13&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N13" s="31" t="str">
@@ -1474,16 +1483,16 @@
         <v>Medium</v>
       </c>
       <c r="O13" s="31" t="str">
-        <f>IF(ISBLANK(I13),"",IF(J13&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="18">
-        <v>9</v>
+      <c r="B14" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>31</v>
@@ -1492,31 +1501,31 @@
         <v>34</v>
       </c>
       <c r="E14" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G14" s="17">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="H14" s="17">
-        <v>30</v>
-      </c>
-      <c r="I14" s="17">
-        <v>0.28867513459481292</v>
+        <v>10</v>
+      </c>
+      <c r="I14" s="43">
+        <v>0.1193524790065721</v>
       </c>
       <c r="J14" s="17">
-        <v>4.2769472400546932E-2</v>
+        <v>0.64577567683708237</v>
       </c>
       <c r="K14" s="17">
-        <v>0.37171435842914707</v>
+        <v>0.14864172138019549</v>
       </c>
       <c r="L14" s="17">
-        <v>4.3116723587406078E-2</v>
+        <v>0.68193556386864729</v>
       </c>
       <c r="M14" s="30" t="str">
-        <f>IF(ISBLANK(I14),"",IF(AND(D14="negative",I14&lt;0),"y",IF(AND(D14="positive",I14&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N14" s="31" t="str">
@@ -1524,16 +1533,16 @@
         <v>Small</v>
       </c>
       <c r="O14" s="31" t="str">
-        <f>IF(ISBLANK(I14),"",IF(J14&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18">
-        <v>9</v>
+      <c r="B15" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>31</v>
@@ -1542,31 +1551,31 @@
         <v>34</v>
       </c>
       <c r="E15" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G15" s="17">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="H15" s="17">
-        <v>30</v>
-      </c>
-      <c r="I15" s="17">
-        <v>0.28465018844122308</v>
+        <v>10</v>
+      </c>
+      <c r="I15" s="43">
+        <v>0.16709347060920099</v>
       </c>
       <c r="J15" s="17">
-        <v>4.660031288457147E-2</v>
+        <v>0.51990361734558355</v>
       </c>
       <c r="K15" s="17">
-        <v>0.35448340067936168</v>
+        <v>0.27250982253035838</v>
       </c>
       <c r="L15" s="17">
-        <v>5.4602722383488088E-2</v>
+        <v>0.44621564369007899</v>
       </c>
       <c r="M15" s="30" t="str">
-        <f>IF(ISBLANK(I15),"",IF(AND(D15="negative",I15&lt;0),"y",IF(AND(D15="positive",I15&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N15" s="31" t="str">
@@ -1574,16 +1583,16 @@
         <v>Small</v>
       </c>
       <c r="O15" s="31" t="str">
-        <f>IF(ISBLANK(I15),"",IF(J15&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="18">
-        <v>9</v>
+      <c r="B16" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>32</v>
@@ -1592,31 +1601,31 @@
         <v>35</v>
       </c>
       <c r="E16" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="G16" s="17">
-        <v>108</v>
+        <v>71</v>
       </c>
       <c r="H16" s="17">
-        <v>30</v>
-      </c>
-      <c r="I16" s="17">
-        <v>-0.3462790510727774</v>
+        <v>10</v>
+      </c>
+      <c r="I16" s="43">
+        <v>-0.35805743701971637</v>
       </c>
       <c r="J16" s="17">
-        <v>1.4781425524297349E-2</v>
+        <v>0.16792075329459241</v>
       </c>
       <c r="K16" s="17">
-        <v>-0.41908679900098411</v>
+        <v>-0.47069878437061913</v>
       </c>
       <c r="L16" s="17">
-        <v>2.1157287218488061E-2</v>
+        <v>0.1697475039817557</v>
       </c>
       <c r="M16" s="30" t="str">
-        <f>IF(ISBLANK(I16),"",IF(AND(D16="negative",I16&lt;0),"y",IF(AND(D16="positive",I16&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N16" s="31" t="str">
@@ -1624,8 +1633,8 @@
         <v>Medium</v>
       </c>
       <c r="O16" s="31" t="str">
-        <f>IF(ISBLANK(I16),"",IF(J16&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1653,20 +1662,20 @@
       <c r="H17" s="19">
         <v>16</v>
       </c>
-      <c r="I17" s="19">
-        <v>-0.1626978433639921</v>
+      <c r="I17" s="44">
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J17" s="19">
-        <v>0.40437459037730811</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K17" s="19">
-        <v>-0.25007261109650641</v>
+        <v>-0.25760491865965418</v>
       </c>
       <c r="L17" s="19">
-        <v>0.35024692329134183</v>
+        <v>0.33543451842856847</v>
       </c>
       <c r="M17" s="32" t="str">
-        <f>IF(ISBLANK(I17),"",IF(AND(D17="negative",I17&lt;0),"y",IF(AND(D17="positive",I17&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N17" s="33" t="str">
@@ -1674,8 +1683,8 @@
         <v>Small</v>
       </c>
       <c r="O17" s="33" t="str">
-        <f>IF(ISBLANK(I17),"",IF(J17&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1703,20 +1712,20 @@
       <c r="H18" s="19">
         <v>16</v>
       </c>
-      <c r="I18" s="19">
-        <v>-0.1988529196671015</v>
+      <c r="I18" s="44">
+        <v>-0.18077538151554681</v>
       </c>
       <c r="J18" s="19">
-        <v>0.30814110145026219</v>
+        <v>0.35419549047641641</v>
       </c>
       <c r="K18" s="19">
-        <v>-0.27417599529857928</v>
+        <v>-0.26664368773543162</v>
       </c>
       <c r="L18" s="19">
-        <v>0.30413535547603471</v>
+        <v>0.31814146487031808</v>
       </c>
       <c r="M18" s="32" t="str">
-        <f>IF(ISBLANK(I18),"",IF(AND(D18="negative",I18&lt;0),"y",IF(AND(D18="positive",I18&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N18" s="33" t="str">
@@ -1724,8 +1733,8 @@
         <v>Small</v>
       </c>
       <c r="O18" s="33" t="str">
-        <f>IF(ISBLANK(I18),"",IF(J18&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="19" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1753,20 +1762,20 @@
       <c r="H19" s="19">
         <v>16</v>
       </c>
-      <c r="I19" s="19">
-        <v>0.37214337343798642</v>
+      <c r="I19" s="44">
+        <v>0.35399003814832852</v>
       </c>
       <c r="J19" s="19">
-        <v>5.7299015704164173E-2</v>
+        <v>7.0561368518920295E-2</v>
       </c>
       <c r="K19" s="19">
-        <v>0.44397949108629498</v>
+        <v>0.43418028330340558</v>
       </c>
       <c r="L19" s="19">
-        <v>8.4931221002269242E-2</v>
+        <v>9.2881780630843944E-2</v>
       </c>
       <c r="M19" s="32" t="str">
-        <f>IF(ISBLANK(I19),"",IF(AND(D19="negative",I19&lt;0),"y",IF(AND(D19="positive",I19&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N19" s="33" t="str">
@@ -1774,8 +1783,8 @@
         <v>Medium</v>
       </c>
       <c r="O19" s="33" t="str">
-        <f>IF(ISBLANK(I19),"",IF(J19&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="20" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1803,20 +1812,20 @@
       <c r="H20" s="19">
         <v>16</v>
       </c>
-      <c r="I20" s="19">
+      <c r="I20" s="44">
         <v>-0.1647705109143269</v>
       </c>
       <c r="J20" s="19">
         <v>0.40275465389762488</v>
       </c>
       <c r="K20" s="19">
-        <v>-0.23419134846990361</v>
+        <v>-0.2493004677260264</v>
       </c>
       <c r="L20" s="19">
-        <v>0.38265747367004138</v>
+        <v>0.35178584403845531</v>
       </c>
       <c r="M20" s="32" t="str">
-        <f>IF(ISBLANK(I20),"",IF(AND(D20="negative",I20&lt;0),"y",IF(AND(D20="positive",I20&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N20" s="33" t="str">
@@ -1824,8 +1833,8 @@
         <v>Small</v>
       </c>
       <c r="O20" s="33" t="str">
-        <f>IF(ISBLANK(I20),"",IF(J20&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="21" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -1853,20 +1862,20 @@
       <c r="H21" s="19">
         <v>16</v>
       </c>
-      <c r="I21" s="19">
+      <c r="I21" s="44">
         <v>-0.1265427670608828</v>
       </c>
       <c r="J21" s="19">
         <v>0.51663737981598823</v>
       </c>
       <c r="K21" s="19">
-        <v>-0.15968492033873299</v>
+        <v>-0.1491396897503261</v>
       </c>
       <c r="L21" s="19">
-        <v>0.55469599227334498</v>
+        <v>0.58145132599759985</v>
       </c>
       <c r="M21" s="32" t="str">
-        <f>IF(ISBLANK(I21),"",IF(AND(D21="negative",I21&lt;0),"y",IF(AND(D21="positive",I21&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N21" s="33" t="str">
@@ -1874,8 +1883,8 @@
         <v>Small</v>
       </c>
       <c r="O21" s="33" t="str">
-        <f>IF(ISBLANK(I21),"",IF(J21&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
@@ -2073,7 +2082,7 @@
         <v>0.20932509565963231</v>
       </c>
       <c r="M2" s="22" t="str">
-        <f>IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
         <v>y</v>
       </c>
       <c r="N2" s="23" t="str">
@@ -2081,7 +2090,7 @@
         <v>Small</v>
       </c>
       <c r="O2" s="23" t="str">
-        <f>IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
+        <f t="shared" ref="O2:O21" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
         <v>n</v>
       </c>
     </row>
@@ -2123,7 +2132,7 @@
         <v>0.13637641008504059</v>
       </c>
       <c r="M3" s="22" t="str">
-        <f>IF(ISBLANK(I3),"",IF(AND(D3="negative",I3&lt;0),"y",IF(AND(D3="positive",I3&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N3" s="23" t="str">
@@ -2131,7 +2140,7 @@
         <v>Small</v>
       </c>
       <c r="O3" s="23" t="str">
-        <f>IF(ISBLANK(I3),"",IF(J3&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2173,7 +2182,7 @@
         <v>0.19405167261558409</v>
       </c>
       <c r="M4" s="22" t="str">
-        <f>IF(ISBLANK(I4),"",IF(AND(D4="negative",I4&lt;0),"y",IF(AND(D4="positive",I4&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N4" s="23" t="str">
@@ -2181,7 +2190,7 @@
         <v>Small</v>
       </c>
       <c r="O4" s="23" t="str">
-        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2211,7 +2220,7 @@
         <v>12</v>
       </c>
       <c r="M5" s="24" t="str">
-        <f>IF(ISBLANK(I5),"",IF(AND(D5="negative",I5&lt;0),"y",IF(AND(D5="positive",I5&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N5" s="25" t="str">
@@ -2219,7 +2228,7 @@
         <v/>
       </c>
       <c r="O5" s="25" t="str">
-        <f>IF(ISBLANK(I5),"",IF(J5&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2249,7 +2258,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="24" t="str">
-        <f>IF(ISBLANK(I6),"",IF(AND(D6="negative",I6&lt;0),"y",IF(AND(D6="positive",I6&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N6" s="25" t="str">
@@ -2257,7 +2266,7 @@
         <v/>
       </c>
       <c r="O6" s="25" t="str">
-        <f>IF(ISBLANK(I6),"",IF(J6&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q6" s="9"/>
@@ -2290,7 +2299,7 @@
         <v>12</v>
       </c>
       <c r="M7" s="24" t="str">
-        <f>IF(ISBLANK(I7),"",IF(AND(D7="negative",I7&lt;0),"y",IF(AND(D7="positive",I7&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" s="25" t="str">
@@ -2298,7 +2307,7 @@
         <v/>
       </c>
       <c r="O7" s="25" t="str">
-        <f>IF(ISBLANK(I7),"",IF(J7&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q7" s="10"/>
@@ -2331,7 +2340,7 @@
         <v>12</v>
       </c>
       <c r="M8" s="24" t="str">
-        <f>IF(ISBLANK(I8),"",IF(AND(D8="negative",I8&lt;0),"y",IF(AND(D8="positive",I8&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N8" s="25" t="str">
@@ -2339,7 +2348,7 @@
         <v/>
       </c>
       <c r="O8" s="25" t="str">
-        <f>IF(ISBLANK(I8),"",IF(J8&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q8" s="10"/>
@@ -2384,7 +2393,7 @@
         <v>3.7567205497513649E-3</v>
       </c>
       <c r="M9" s="26" t="str">
-        <f>IF(ISBLANK(I9),"",IF(AND(D9="negative",I9&lt;0),"y",IF(AND(D9="positive",I9&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N9" s="27" t="str">
@@ -2392,7 +2401,7 @@
         <v>Small</v>
       </c>
       <c r="O9" s="27" t="str">
-        <f>IF(ISBLANK(I9),"",IF(J9&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
       <c r="Q9" s="13"/>
@@ -2437,7 +2446,7 @@
         <v>0.88084937555910936</v>
       </c>
       <c r="M10" s="28" t="str">
-        <f>IF(ISBLANK(I10),"",IF(AND(D10="negative",I10&lt;0),"y",IF(AND(D10="positive",I10&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N10" s="29" t="str">
@@ -2445,7 +2454,7 @@
         <v>None</v>
       </c>
       <c r="O10" s="29" t="str">
-        <f>IF(ISBLANK(I10),"",IF(J10&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q10" s="16"/>
@@ -2490,7 +2499,7 @@
         <v>0.84666464123863983</v>
       </c>
       <c r="M11" s="28" t="str">
-        <f>IF(ISBLANK(I11),"",IF(AND(D11="negative",I11&lt;0),"y",IF(AND(D11="positive",I11&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N11" s="29" t="str">
@@ -2498,7 +2507,7 @@
         <v>None</v>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF(ISBLANK(I11),"",IF(J11&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2540,7 +2549,7 @@
         <v>2.7488825966879269E-2</v>
       </c>
       <c r="M12" s="28" t="str">
-        <f>IF(ISBLANK(I12),"",IF(AND(D12="negative",I12&lt;0),"y",IF(AND(D12="positive",I12&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N12" s="29" t="str">
@@ -2548,7 +2557,7 @@
         <v>Small</v>
       </c>
       <c r="O12" s="29" t="str">
-        <f>IF(ISBLANK(I12),"",IF(J12&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
     </row>
@@ -2590,7 +2599,7 @@
         <v>0.32836965842449101</v>
       </c>
       <c r="M13" s="30" t="str">
-        <f>IF(ISBLANK(I13),"",IF(AND(D13="negative",I13&lt;0),"y",IF(AND(D13="positive",I13&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N13" s="31" t="str">
@@ -2598,7 +2607,7 @@
         <v>Small</v>
       </c>
       <c r="O13" s="31" t="str">
-        <f>IF(ISBLANK(I13),"",IF(J13&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2640,7 +2649,7 @@
         <v>0.17978258043948159</v>
       </c>
       <c r="M14" s="30" t="str">
-        <f>IF(ISBLANK(I14),"",IF(AND(D14="negative",I14&lt;0),"y",IF(AND(D14="positive",I14&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N14" s="31" t="str">
@@ -2648,7 +2657,7 @@
         <v>Small</v>
       </c>
       <c r="O14" s="31" t="str">
-        <f>IF(ISBLANK(I14),"",IF(J14&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2690,7 +2699,7 @@
         <v>0.18660467276809919</v>
       </c>
       <c r="M15" s="30" t="str">
-        <f>IF(ISBLANK(I15),"",IF(AND(D15="negative",I15&lt;0),"y",IF(AND(D15="positive",I15&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N15" s="31" t="str">
@@ -2698,7 +2707,7 @@
         <v>Small</v>
       </c>
       <c r="O15" s="31" t="str">
-        <f>IF(ISBLANK(I15),"",IF(J15&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2740,7 +2749,7 @@
         <v>0.67966876801064502</v>
       </c>
       <c r="M16" s="30" t="str">
-        <f>IF(ISBLANK(I16),"",IF(AND(D16="negative",I16&lt;0),"y",IF(AND(D16="positive",I16&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N16" s="31" t="str">
@@ -2748,7 +2757,7 @@
         <v>None</v>
       </c>
       <c r="O16" s="31" t="str">
-        <f>IF(ISBLANK(I16),"",IF(J16&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2790,7 +2799,7 @@
         <v>0.65376710935384819</v>
       </c>
       <c r="M17" s="32" t="str">
-        <f>IF(ISBLANK(I17),"",IF(AND(D17="negative",I17&lt;0),"y",IF(AND(D17="positive",I17&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N17" s="33" t="str">
@@ -2798,7 +2807,7 @@
         <v>Small</v>
       </c>
       <c r="O17" s="33" t="str">
-        <f>IF(ISBLANK(I17),"",IF(J17&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2840,7 +2849,7 @@
         <v>0.94909603273704102</v>
       </c>
       <c r="M18" s="32" t="str">
-        <f>IF(ISBLANK(I18),"",IF(AND(D18="negative",I18&lt;0),"y",IF(AND(D18="positive",I18&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N18" s="33" t="str">
@@ -2848,7 +2857,7 @@
         <v>None</v>
       </c>
       <c r="O18" s="33" t="str">
-        <f>IF(ISBLANK(I18),"",IF(J18&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2890,7 +2899,7 @@
         <v>0.21158246186830859</v>
       </c>
       <c r="M19" s="32" t="str">
-        <f>IF(ISBLANK(I19),"",IF(AND(D19="negative",I19&lt;0),"y",IF(AND(D19="positive",I19&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N19" s="33" t="str">
@@ -2898,7 +2907,7 @@
         <v>Small</v>
       </c>
       <c r="O19" s="33" t="str">
-        <f>IF(ISBLANK(I19),"",IF(J19&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2940,7 +2949,7 @@
         <v>0.4771333722542902</v>
       </c>
       <c r="M20" s="32" t="str">
-        <f>IF(ISBLANK(I20),"",IF(AND(D20="negative",I20&lt;0),"y",IF(AND(D20="positive",I20&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N20" s="33" t="str">
@@ -2948,7 +2957,7 @@
         <v>Small</v>
       </c>
       <c r="O20" s="33" t="str">
-        <f>IF(ISBLANK(I20),"",IF(J20&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -2990,7 +2999,7 @@
         <v>0.26690125229506823</v>
       </c>
       <c r="M21" s="32" t="str">
-        <f>IF(ISBLANK(I21),"",IF(AND(D21="negative",I21&lt;0),"y",IF(AND(D21="positive",I21&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N21" s="33" t="str">
@@ -2998,7 +3007,7 @@
         <v>Small</v>
       </c>
       <c r="O21" s="33" t="str">
-        <f>IF(ISBLANK(I21),"",IF(J21&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3195,7 +3204,7 @@
         <v>0.31170668319455619</v>
       </c>
       <c r="M2" s="22" t="str">
-        <f>IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
         <v>y</v>
       </c>
       <c r="N2" s="23" t="str">
@@ -3203,7 +3212,7 @@
         <v>Small</v>
       </c>
       <c r="O2" s="23" t="str">
-        <f>IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
+        <f t="shared" ref="O2:O21" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
         <v>n</v>
       </c>
     </row>
@@ -3245,7 +3254,7 @@
         <v>0.19070138371258061</v>
       </c>
       <c r="M3" s="22" t="str">
-        <f>IF(ISBLANK(I3),"",IF(AND(D3="negative",I3&lt;0),"y",IF(AND(D3="positive",I3&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N3" s="23" t="str">
@@ -3253,7 +3262,7 @@
         <v>Small</v>
       </c>
       <c r="O3" s="23" t="str">
-        <f>IF(ISBLANK(I3),"",IF(J3&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3295,7 +3304,7 @@
         <v>0.26904897632032188</v>
       </c>
       <c r="M4" s="22" t="str">
-        <f>IF(ISBLANK(I4),"",IF(AND(D4="negative",I4&lt;0),"y",IF(AND(D4="positive",I4&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N4" s="23" t="str">
@@ -3303,7 +3312,7 @@
         <v>Small</v>
       </c>
       <c r="O4" s="23" t="str">
-        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3345,7 +3354,7 @@
         <v>0.68484871442737572</v>
       </c>
       <c r="M5" s="24" t="str">
-        <f>IF(ISBLANK(I5),"",IF(AND(D5="negative",I5&lt;0),"y",IF(AND(D5="positive",I5&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N5" s="25" t="str">
@@ -3353,7 +3362,7 @@
         <v>Small</v>
       </c>
       <c r="O5" s="25" t="str">
-        <f>IF(ISBLANK(I5),"",IF(J5&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3395,7 +3404,7 @@
         <v>0.33389313645066021</v>
       </c>
       <c r="M6" s="24" t="str">
-        <f>IF(ISBLANK(I6),"",IF(AND(D6="negative",I6&lt;0),"y",IF(AND(D6="positive",I6&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N6" s="25" t="str">
@@ -3403,7 +3412,7 @@
         <v>Small</v>
       </c>
       <c r="O6" s="25" t="str">
-        <f>IF(ISBLANK(I6),"",IF(J6&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q6" s="9"/>
@@ -3448,7 +3457,7 @@
         <v>0.68484871442737572</v>
       </c>
       <c r="M7" s="24" t="str">
-        <f>IF(ISBLANK(I7),"",IF(AND(D7="negative",I7&lt;0),"y",IF(AND(D7="positive",I7&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N7" s="25" t="str">
@@ -3456,7 +3465,7 @@
         <v>Small</v>
       </c>
       <c r="O7" s="25" t="str">
-        <f>IF(ISBLANK(I7),"",IF(J7&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q7" s="10"/>
@@ -3501,7 +3510,7 @@
         <v>0.33389313645066021</v>
       </c>
       <c r="M8" s="24" t="str">
-        <f>IF(ISBLANK(I8),"",IF(AND(D8="negative",I8&lt;0),"y",IF(AND(D8="positive",I8&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N8" s="25" t="str">
@@ -3509,7 +3518,7 @@
         <v>Small</v>
       </c>
       <c r="O8" s="25" t="str">
-        <f>IF(ISBLANK(I8),"",IF(J8&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q8" s="10"/>
@@ -3554,7 +3563,7 @@
         <v>2.7610565923995401E-2</v>
       </c>
       <c r="M9" s="26" t="str">
-        <f>IF(ISBLANK(I9),"",IF(AND(D9="negative",I9&lt;0),"y",IF(AND(D9="positive",I9&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N9" s="27" t="str">
@@ -3562,7 +3571,7 @@
         <v>Small</v>
       </c>
       <c r="O9" s="27" t="str">
-        <f>IF(ISBLANK(I9),"",IF(J9&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
       <c r="Q9" s="13"/>
@@ -3607,7 +3616,7 @@
         <v>0.33135638533698542</v>
       </c>
       <c r="M10" s="28" t="str">
-        <f>IF(ISBLANK(I10),"",IF(AND(D10="negative",I10&lt;0),"y",IF(AND(D10="positive",I10&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N10" s="29" t="str">
@@ -3615,7 +3624,7 @@
         <v>Small</v>
       </c>
       <c r="O10" s="29" t="str">
-        <f>IF(ISBLANK(I10),"",IF(J10&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q10" s="16"/>
@@ -3660,7 +3669,7 @@
         <v>0.53816988278746214</v>
       </c>
       <c r="M11" s="28" t="str">
-        <f>IF(ISBLANK(I11),"",IF(AND(D11="negative",I11&lt;0),"y",IF(AND(D11="positive",I11&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N11" s="29" t="str">
@@ -3668,7 +3677,7 @@
         <v>None</v>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF(ISBLANK(I11),"",IF(J11&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3710,7 +3719,7 @@
         <v>0.47253953182670588</v>
       </c>
       <c r="M12" s="28" t="str">
-        <f>IF(ISBLANK(I12),"",IF(AND(D12="negative",I12&lt;0),"y",IF(AND(D12="positive",I12&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N12" s="29" t="str">
@@ -3718,7 +3727,7 @@
         <v>None</v>
       </c>
       <c r="O12" s="29" t="str">
-        <f>IF(ISBLANK(I12),"",IF(J12&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3748,7 +3757,7 @@
         <v>30</v>
       </c>
       <c r="M13" s="30" t="str">
-        <f>IF(ISBLANK(I13),"",IF(AND(D13="negative",I13&lt;0),"y",IF(AND(D13="positive",I13&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N13" s="31" t="str">
@@ -3756,7 +3765,7 @@
         <v/>
       </c>
       <c r="O13" s="31" t="str">
-        <f>IF(ISBLANK(I13),"",IF(J13&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3786,7 +3795,7 @@
         <v>30</v>
       </c>
       <c r="M14" s="30" t="str">
-        <f>IF(ISBLANK(I14),"",IF(AND(D14="negative",I14&lt;0),"y",IF(AND(D14="positive",I14&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N14" s="31" t="str">
@@ -3794,7 +3803,7 @@
         <v/>
       </c>
       <c r="O14" s="31" t="str">
-        <f>IF(ISBLANK(I14),"",IF(J14&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3824,7 +3833,7 @@
         <v>30</v>
       </c>
       <c r="M15" s="30" t="str">
-        <f>IF(ISBLANK(I15),"",IF(AND(D15="negative",I15&lt;0),"y",IF(AND(D15="positive",I15&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N15" s="31" t="str">
@@ -3832,7 +3841,7 @@
         <v/>
       </c>
       <c r="O15" s="31" t="str">
-        <f>IF(ISBLANK(I15),"",IF(J15&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3862,7 +3871,7 @@
         <v>30</v>
       </c>
       <c r="M16" s="30" t="str">
-        <f>IF(ISBLANK(I16),"",IF(AND(D16="negative",I16&lt;0),"y",IF(AND(D16="positive",I16&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N16" s="31" t="str">
@@ -3870,7 +3879,7 @@
         <v/>
       </c>
       <c r="O16" s="31" t="str">
-        <f>IF(ISBLANK(I16),"",IF(J16&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -3912,7 +3921,7 @@
         <v>0.68526500553668901</v>
       </c>
       <c r="M17" s="32" t="str">
-        <f>IF(ISBLANK(I17),"",IF(AND(D17="negative",I17&lt;0),"y",IF(AND(D17="positive",I17&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N17" s="33" t="str">
@@ -3920,7 +3929,7 @@
         <v>None</v>
       </c>
       <c r="O17" s="33" t="str">
-        <f>IF(ISBLANK(I17),"",IF(J17&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -3962,7 +3971,7 @@
         <v>0.68526500553668901</v>
       </c>
       <c r="M18" s="32" t="str">
-        <f>IF(ISBLANK(I18),"",IF(AND(D18="negative",I18&lt;0),"y",IF(AND(D18="positive",I18&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N18" s="33" t="str">
@@ -3970,7 +3979,7 @@
         <v>None</v>
       </c>
       <c r="O18" s="33" t="str">
-        <f>IF(ISBLANK(I18),"",IF(J18&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -4012,7 +4021,7 @@
         <v>0.1217337691688223</v>
       </c>
       <c r="M19" s="32" t="str">
-        <f>IF(ISBLANK(I19),"",IF(AND(D19="negative",I19&lt;0),"y",IF(AND(D19="positive",I19&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N19" s="33" t="str">
@@ -4020,7 +4029,7 @@
         <v>Medium</v>
       </c>
       <c r="O19" s="33" t="str">
-        <f>IF(ISBLANK(I19),"",IF(J19&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -4062,7 +4071,7 @@
         <v>1.929785020805572E-2</v>
       </c>
       <c r="M20" s="32" t="str">
-        <f>IF(ISBLANK(I20),"",IF(AND(D20="negative",I20&lt;0),"y",IF(AND(D20="positive",I20&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N20" s="33" t="str">
@@ -4070,7 +4079,7 @@
         <v>Medium</v>
       </c>
       <c r="O20" s="33" t="str">
-        <f>IF(ISBLANK(I20),"",IF(J20&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
     </row>
@@ -4112,7 +4121,7 @@
         <v>0.88786930283188992</v>
       </c>
       <c r="M21" s="32" t="str">
-        <f>IF(ISBLANK(I21),"",IF(AND(D21="negative",I21&lt;0),"y",IF(AND(D21="positive",I21&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N21" s="33" t="str">
@@ -4120,7 +4129,7 @@
         <v>None</v>
       </c>
       <c r="O21" s="33" t="str">
-        <f>IF(ISBLANK(I21),"",IF(J21&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -4210,8 +4219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:S30"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4305,7 +4314,7 @@
         <v>23</v>
       </c>
       <c r="M2" s="22" t="str">
-        <f>IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
         <v/>
       </c>
       <c r="N2" s="23" t="str">
@@ -4313,7 +4322,7 @@
         <v/>
       </c>
       <c r="O2" s="23" t="str">
-        <f>IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
+        <f t="shared" ref="O2:O21" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.01,"**",IF(J2&lt;0.05,"*", "")))</f>
         <v/>
       </c>
     </row>
@@ -4343,7 +4352,7 @@
         <v>23</v>
       </c>
       <c r="M3" s="22" t="str">
-        <f>IF(ISBLANK(I3),"",IF(AND(D3="negative",I3&lt;0),"y",IF(AND(D3="positive",I3&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N3" s="23" t="str">
@@ -4351,7 +4360,7 @@
         <v/>
       </c>
       <c r="O3" s="23" t="str">
-        <f>IF(ISBLANK(I3),"",IF(J3&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -4381,7 +4390,7 @@
         <v>23</v>
       </c>
       <c r="M4" s="22" t="str">
-        <f>IF(ISBLANK(I4),"",IF(AND(D4="negative",I4&lt;0),"y",IF(AND(D4="positive",I4&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N4" s="23" t="str">
@@ -4389,7 +4398,7 @@
         <v/>
       </c>
       <c r="O4" s="23" t="str">
-        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.05,"y","n"))</f>
+        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.01,"**",IF(J4&lt;0.05,"*", "")))</f>
         <v/>
       </c>
     </row>
@@ -4419,7 +4428,7 @@
         <v>12</v>
       </c>
       <c r="M5" s="24" t="str">
-        <f>IF(ISBLANK(I5),"",IF(AND(D5="negative",I5&lt;0),"y",IF(AND(D5="positive",I5&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N5" s="25" t="str">
@@ -4427,7 +4436,7 @@
         <v/>
       </c>
       <c r="O5" s="25" t="str">
-        <f>IF(ISBLANK(I5),"",IF(J5&lt;0.05,"y","n"))</f>
+        <f t="shared" ref="O5:O21" si="2">IF(ISBLANK(I5),"",IF(J5&lt;0.01,"**",IF(J5&lt;0.05,"*", "")))</f>
         <v/>
       </c>
     </row>
@@ -4457,7 +4466,7 @@
         <v>12</v>
       </c>
       <c r="M6" s="24" t="str">
-        <f>IF(ISBLANK(I6),"",IF(AND(D6="negative",I6&lt;0),"y",IF(AND(D6="positive",I6&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N6" s="25" t="str">
@@ -4465,7 +4474,7 @@
         <v/>
       </c>
       <c r="O6" s="25" t="str">
-        <f>IF(ISBLANK(I6),"",IF(J6&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q6" s="9"/>
@@ -4498,7 +4507,7 @@
         <v>12</v>
       </c>
       <c r="M7" s="24" t="str">
-        <f>IF(ISBLANK(I7),"",IF(AND(D7="negative",I7&lt;0),"y",IF(AND(D7="positive",I7&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N7" s="25" t="str">
@@ -4506,7 +4515,7 @@
         <v/>
       </c>
       <c r="O7" s="25" t="str">
-        <f>IF(ISBLANK(I7),"",IF(J7&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q7" s="10"/>
@@ -4539,7 +4548,7 @@
         <v>12</v>
       </c>
       <c r="M8" s="24" t="str">
-        <f>IF(ISBLANK(I8),"",IF(AND(D8="negative",I8&lt;0),"y",IF(AND(D8="positive",I8&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N8" s="25" t="str">
@@ -4547,7 +4556,7 @@
         <v/>
       </c>
       <c r="O8" s="25" t="str">
-        <f>IF(ISBLANK(I8),"",IF(J8&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="Q8" s="10"/>
@@ -4592,7 +4601,7 @@
         <v>0.1090548020620709</v>
       </c>
       <c r="M9" s="26" t="str">
-        <f>IF(ISBLANK(I9),"",IF(AND(D9="negative",I9&lt;0),"y",IF(AND(D9="positive",I9&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N9" s="27" t="str">
@@ -4600,8 +4609,8 @@
         <v>Small</v>
       </c>
       <c r="O9" s="27" t="str">
-        <f>IF(ISBLANK(I9),"",IF(J9&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
@@ -4624,28 +4633,28 @@
         <v>50</v>
       </c>
       <c r="F10" s="14">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G10" s="14">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H10" s="14">
         <v>50</v>
       </c>
       <c r="I10" s="14">
-        <v>-1.7966219332967059E-2</v>
+        <v>-4.0010884441053322E-3</v>
       </c>
       <c r="J10" s="14">
-        <v>0.88314281706898357</v>
+        <v>0.97393749824887355</v>
       </c>
       <c r="K10" s="14">
-        <v>-1.9415750760330759E-2</v>
+        <v>-4.0145445731910407E-3</v>
       </c>
       <c r="L10" s="14">
-        <v>0.89353687009819049</v>
+        <v>0.97792597559776806</v>
       </c>
       <c r="M10" s="28" t="str">
-        <f>IF(ISBLANK(I10),"",IF(AND(D10="negative",I10&lt;0),"y",IF(AND(D10="positive",I10&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N10" s="29" t="str">
@@ -4653,8 +4662,8 @@
         <v>None</v>
       </c>
       <c r="O10" s="29" t="str">
-        <f>IF(ISBLANK(I10),"",IF(J10&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
@@ -4677,28 +4686,28 @@
         <v>50</v>
       </c>
       <c r="F11" s="14">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G11" s="14">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H11" s="14">
         <v>50</v>
       </c>
       <c r="I11" s="14">
-        <v>-2.0733912312975989E-2</v>
+        <v>-1.8889590382011531E-2</v>
       </c>
       <c r="J11" s="14">
-        <v>0.85903161553489027</v>
+        <v>0.8717029852220165</v>
       </c>
       <c r="K11" s="14">
-        <v>-2.339586347864377E-2</v>
+        <v>-2.2061548434927108E-2</v>
       </c>
       <c r="L11" s="14">
-        <v>0.87187961817406379</v>
+        <v>0.87913055885863645</v>
       </c>
       <c r="M11" s="28" t="str">
-        <f>IF(ISBLANK(I11),"",IF(AND(D11="negative",I11&lt;0),"y",IF(AND(D11="positive",I11&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N11" s="29" t="str">
@@ -4706,8 +4715,8 @@
         <v>None</v>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF(ISBLANK(I11),"",IF(J11&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="12" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.2">
@@ -4727,28 +4736,28 @@
         <v>50</v>
       </c>
       <c r="F12" s="14">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G12" s="14">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="H12" s="14">
         <v>50</v>
       </c>
       <c r="I12" s="14">
-        <v>-0.24894627719055901</v>
+        <v>-0.24760641624976251</v>
       </c>
       <c r="J12" s="14">
-        <v>3.1843356716153078E-2</v>
+        <v>3.3114212859699399E-2</v>
       </c>
       <c r="K12" s="14">
-        <v>-0.31078029944537922</v>
+        <v>-0.30991275370518351</v>
       </c>
       <c r="L12" s="14">
-        <v>2.8043445822604571E-2</v>
+        <v>2.850794708171081E-2</v>
       </c>
       <c r="M12" s="28" t="str">
-        <f>IF(ISBLANK(I12),"",IF(AND(D12="negative",I12&lt;0),"y",IF(AND(D12="positive",I12&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N12" s="29" t="str">
@@ -4756,16 +4765,16 @@
         <v>Small</v>
       </c>
       <c r="O12" s="29" t="str">
-        <f>IF(ISBLANK(I12),"",IF(J12&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v>*</v>
       </c>
     </row>
     <row r="13" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="18">
-        <v>9</v>
+      <c r="B13" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C13" s="17" t="s">
         <v>30</v>
@@ -4774,31 +4783,31 @@
         <v>34</v>
       </c>
       <c r="E13" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F13" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G13" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H13" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I13" s="17">
-        <v>-0.153506269493634</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J13" s="17">
-        <v>0.31976301166779852</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K13" s="17">
-        <v>-0.1847566494939108</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L13" s="17">
-        <v>0.32836965842449101</v>
+        <v>0.42602444842854259</v>
       </c>
       <c r="M13" s="30" t="str">
-        <f>IF(ISBLANK(I13),"",IF(AND(D13="negative",I13&lt;0),"y",IF(AND(D13="positive",I13&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N13" s="31" t="str">
@@ -4806,16 +4815,16 @@
         <v>Small</v>
       </c>
       <c r="O13" s="31" t="str">
-        <f>IF(ISBLANK(I13),"",IF(J13&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="14" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="18">
-        <v>9</v>
+      <c r="B14" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C14" s="17" t="s">
         <v>31</v>
@@ -4824,31 +4833,31 @@
         <v>34</v>
       </c>
       <c r="E14" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F14" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G14" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H14" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I14" s="17">
-        <v>0.2815332554724217</v>
+        <v>0.1217161238900369</v>
       </c>
       <c r="J14" s="17">
-        <v>6.8615535355580695E-2</v>
+        <v>0.66981535759941657</v>
       </c>
       <c r="K14" s="17">
-        <v>0.33814060970304249</v>
+        <v>0.1421338109037403</v>
       </c>
       <c r="L14" s="17">
-        <v>6.7604521629823694E-2</v>
+        <v>0.69528768540126551</v>
       </c>
       <c r="M14" s="30" t="str">
-        <f>IF(ISBLANK(I14),"",IF(AND(D14="negative",I14&lt;0),"y",IF(AND(D14="positive",I14&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N14" s="31" t="str">
@@ -4856,16 +4865,16 @@
         <v>Small</v>
       </c>
       <c r="O14" s="31" t="str">
-        <f>IF(ISBLANK(I14),"",IF(J14&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="15" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="18">
-        <v>9</v>
+      <c r="B15" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C15" s="17" t="s">
         <v>31</v>
@@ -4874,48 +4883,48 @@
         <v>34</v>
       </c>
       <c r="E15" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F15" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G15" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H15" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I15" s="17">
-        <v>0.3157348151855433</v>
+        <v>0.24343224778007391</v>
       </c>
       <c r="J15" s="17">
-        <v>4.1947627723575583E-2</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K15" s="17">
-        <v>0.37771162574734057</v>
+        <v>0.28426762180748061</v>
       </c>
       <c r="L15" s="17">
-        <v>3.9605634003798212E-2</v>
+        <v>0.42602444842854259</v>
       </c>
       <c r="M15" s="30" t="str">
-        <f>IF(ISBLANK(I15),"",IF(AND(D15="negative",I15&lt;0),"y",IF(AND(D15="positive",I15&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N15" s="31" t="str">
         <f>IF(ISBLANK(I15),"",LOOKUP(ABS(I15),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v>Medium</v>
+        <v>Small</v>
       </c>
       <c r="O15" s="31" t="str">
-        <f>IF(ISBLANK(I15),"",IF(J15&lt;0.05,"y","n"))</f>
-        <v>y</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="16" spans="1:19" s="17" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="18">
-        <v>9</v>
+      <c r="B16" s="18" t="s">
+        <v>54</v>
       </c>
       <c r="C16" s="17" t="s">
         <v>32</v>
@@ -4924,31 +4933,31 @@
         <v>35</v>
       </c>
       <c r="E16" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="F16" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G16" s="17">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="H16" s="17">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="I16" s="17">
-        <v>-0.14354272032581639</v>
+        <v>-0.24343224778007391</v>
       </c>
       <c r="J16" s="17">
-        <v>0.35168068279855269</v>
+        <v>0.39376863464299272</v>
       </c>
       <c r="K16" s="17">
-        <v>-0.17294443123341199</v>
+        <v>-0.28426762180748061</v>
       </c>
       <c r="L16" s="17">
-        <v>0.36075974854167298</v>
+        <v>0.42602444842854259</v>
       </c>
       <c r="M16" s="30" t="str">
-        <f>IF(ISBLANK(I16),"",IF(AND(D16="negative",I16&lt;0),"y",IF(AND(D16="positive",I16&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N16" s="31" t="str">
@@ -4956,8 +4965,8 @@
         <v>Small</v>
       </c>
       <c r="O16" s="31" t="str">
-        <f>IF(ISBLANK(I16),"",IF(J16&lt;0.05,"y","n"))</f>
-        <v>n</v>
+        <f t="shared" si="2"/>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:15" s="19" customFormat="1" x14ac:dyDescent="0.2">
@@ -4977,24 +4986,36 @@
         <v>16</v>
       </c>
       <c r="F17" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="19">
         <v>16</v>
       </c>
+      <c r="I17" s="19">
+        <v>-0.35355339059327368</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0.1037416782365415</v>
+      </c>
+      <c r="K17" s="19">
+        <v>-0.42008402520840288</v>
+      </c>
+      <c r="L17" s="19">
+        <v>0.105228057983522</v>
+      </c>
       <c r="M17" s="32" t="str">
-        <f>IF(ISBLANK(I17),"",IF(AND(D17="negative",I17&lt;0),"y",IF(AND(D17="positive",I17&gt;0), "y","n")))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="N17" s="33" t="str">
         <f>IF(ISBLANK(I17),"",LOOKUP(ABS(I17),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v/>
+        <v>Medium</v>
       </c>
       <c r="O17" s="33" t="str">
-        <f>IF(ISBLANK(I17),"",IF(J17&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5015,24 +5036,36 @@
         <v>16</v>
       </c>
       <c r="F18" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G18" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H18" s="19">
         <v>16</v>
       </c>
+      <c r="I18" s="19">
+        <v>-0.16499158227686109</v>
+      </c>
+      <c r="J18" s="19">
+        <v>0.4476990724652935</v>
+      </c>
+      <c r="K18" s="19">
+        <v>-0.19603921176392139</v>
+      </c>
+      <c r="L18" s="19">
+        <v>0.4668248490265503</v>
+      </c>
       <c r="M18" s="32" t="str">
-        <f>IF(ISBLANK(I18),"",IF(AND(D18="negative",I18&lt;0),"y",IF(AND(D18="positive",I18&gt;0), "y","n")))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="N18" s="33" t="str">
         <f>IF(ISBLANK(I18),"",LOOKUP(ABS(I18),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v/>
+        <v>Small</v>
       </c>
       <c r="O18" s="33" t="str">
-        <f>IF(ISBLANK(I18),"",IF(J18&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5053,24 +5086,36 @@
         <v>16</v>
       </c>
       <c r="F19" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G19" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="19">
         <v>16</v>
       </c>
+      <c r="I19" s="19">
+        <v>2.3669053416557541E-2</v>
+      </c>
+      <c r="J19" s="19">
+        <v>0.91356333033778614</v>
+      </c>
+      <c r="K19" s="19">
+        <v>2.802621677476181E-2</v>
+      </c>
+      <c r="L19" s="19">
+        <v>0.91793879859999294</v>
+      </c>
       <c r="M19" s="32" t="str">
-        <f>IF(ISBLANK(I19),"",IF(AND(D19="negative",I19&lt;0),"y",IF(AND(D19="positive",I19&gt;0), "y","n")))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="N19" s="33" t="str">
         <f>IF(ISBLANK(I19),"",LOOKUP(ABS(I19),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v/>
+        <v>None</v>
       </c>
       <c r="O19" s="33" t="str">
-        <f>IF(ISBLANK(I19),"",IF(J19&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5091,24 +5136,36 @@
         <v>16</v>
       </c>
       <c r="F20" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="19">
         <v>16</v>
       </c>
+      <c r="I20" s="19">
+        <v>-0.26257545381445868</v>
+      </c>
+      <c r="J20" s="19">
+        <v>0.23144602710389381</v>
+      </c>
+      <c r="K20" s="19">
+        <v>-0.30897169910547828</v>
+      </c>
+      <c r="L20" s="19">
+        <v>0.24426062662249609</v>
+      </c>
       <c r="M20" s="32" t="str">
-        <f>IF(ISBLANK(I20),"",IF(AND(D20="negative",I20&lt;0),"y",IF(AND(D20="positive",I20&gt;0), "y","n")))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="N20" s="33" t="str">
         <f>IF(ISBLANK(I20),"",LOOKUP(ABS(I20),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v/>
+        <v>Small</v>
       </c>
       <c r="O20" s="33" t="str">
-        <f>IF(ISBLANK(I20),"",IF(J20&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5129,24 +5186,36 @@
         <v>16</v>
       </c>
       <c r="F21" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21" s="19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="19">
         <v>16</v>
       </c>
+      <c r="I21" s="19">
+        <v>0.25927248643506751</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0.2328233516916538</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0.30806161848616209</v>
+      </c>
+      <c r="L21" s="19">
+        <v>0.2457251662216493</v>
+      </c>
       <c r="M21" s="32" t="str">
-        <f>IF(ISBLANK(I21),"",IF(AND(D21="negative",I21&lt;0),"y",IF(AND(D21="positive",I21&gt;0), "y","n")))</f>
-        <v/>
+        <f t="shared" si="0"/>
+        <v>y</v>
       </c>
       <c r="N21" s="33" t="str">
         <f>IF(ISBLANK(I21),"",LOOKUP(ABS(I21),all_tools!$Q$7:$Q$10,all_tools!$S$7:$S$10))</f>
-        <v/>
+        <v>Small</v>
       </c>
       <c r="O21" s="33" t="str">
-        <f>IF(ISBLANK(I21),"",IF(J21&lt;0.05,"y","n"))</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
     </row>
@@ -5156,7 +5225,7 @@
       </c>
       <c r="M23" s="3">
         <f>M24-COUNTBLANK(M2:M21)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -5174,7 +5243,7 @@
       </c>
       <c r="M25" s="3">
         <f>COUNTIF(M2:M21,"y")</f>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -5183,7 +5252,7 @@
       </c>
       <c r="M26" s="38">
         <f>M25/M24</f>
-        <v>0.2</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -5192,7 +5261,7 @@
       </c>
       <c r="M27" s="3">
         <f>M25-COUNTIFS(M2:M21,"y",N2:N21,"None")</f>
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -5201,7 +5270,7 @@
       </c>
       <c r="M28" s="38">
         <f>M27/M24</f>
-        <v>0.1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -5343,7 +5412,7 @@
         <v>0.157096814687567</v>
       </c>
       <c r="M2" s="22" t="str">
-        <f>IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
+        <f t="shared" ref="M2:M21" si="0">IF(ISBLANK(I2),"",IF(AND(D2="negative",I2&lt;0),"y",IF(AND(D2="positive",I2&gt;0), "y","n")))</f>
         <v>y</v>
       </c>
       <c r="N2" s="23" t="str">
@@ -5351,7 +5420,7 @@
         <v>Small</v>
       </c>
       <c r="O2" s="23" t="str">
-        <f>IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
+        <f t="shared" ref="O2:O21" si="1">IF(ISBLANK(I2),"",IF(J2&lt;0.05,"y","n"))</f>
         <v>n</v>
       </c>
     </row>
@@ -5393,7 +5462,7 @@
         <v>3.2426785472927828E-2</v>
       </c>
       <c r="M3" s="22" t="str">
-        <f>IF(ISBLANK(I3),"",IF(AND(D3="negative",I3&lt;0),"y",IF(AND(D3="positive",I3&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N3" s="23" t="str">
@@ -5401,7 +5470,7 @@
         <v>Medium</v>
       </c>
       <c r="O3" s="23" t="str">
-        <f>IF(ISBLANK(I3),"",IF(J3&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
     </row>
@@ -5443,7 +5512,7 @@
         <v>2.9842113749669798E-2</v>
       </c>
       <c r="M4" s="22" t="str">
-        <f>IF(ISBLANK(I4),"",IF(AND(D4="negative",I4&lt;0),"y",IF(AND(D4="positive",I4&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N4" s="23" t="str">
@@ -5451,7 +5520,7 @@
         <v>Medium</v>
       </c>
       <c r="O4" s="23" t="str">
-        <f>IF(ISBLANK(I4),"",IF(J4&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
     </row>
@@ -5493,7 +5562,7 @@
         <v>0.52130971968204398</v>
       </c>
       <c r="M5" s="24" t="str">
-        <f>IF(ISBLANK(I5),"",IF(AND(D5="negative",I5&lt;0),"y",IF(AND(D5="positive",I5&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N5" s="25" t="str">
@@ -5501,7 +5570,7 @@
         <v>Small</v>
       </c>
       <c r="O5" s="25" t="str">
-        <f>IF(ISBLANK(I5),"",IF(J5&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -5543,7 +5612,7 @@
         <v>0.4451488240391529</v>
       </c>
       <c r="M6" s="24" t="str">
-        <f>IF(ISBLANK(I6),"",IF(AND(D6="negative",I6&lt;0),"y",IF(AND(D6="positive",I6&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N6" s="25" t="str">
@@ -5551,7 +5620,7 @@
         <v>Small</v>
       </c>
       <c r="O6" s="25" t="str">
-        <f>IF(ISBLANK(I6),"",IF(J6&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q6" s="9"/>
@@ -5596,7 +5665,7 @@
         <v>6.0434956200926593E-2</v>
       </c>
       <c r="M7" s="24" t="str">
-        <f>IF(ISBLANK(I7),"",IF(AND(D7="negative",I7&lt;0),"y",IF(AND(D7="positive",I7&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N7" s="25" t="str">
@@ -5604,7 +5673,7 @@
         <v>Medium</v>
       </c>
       <c r="O7" s="25" t="str">
-        <f>IF(ISBLANK(I7),"",IF(J7&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>y</v>
       </c>
       <c r="Q7" s="10"/>
@@ -5649,7 +5718,7 @@
         <v>0.19305349764481941</v>
       </c>
       <c r="M8" s="24" t="str">
-        <f>IF(ISBLANK(I8),"",IF(AND(D8="negative",I8&lt;0),"y",IF(AND(D8="positive",I8&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N8" s="25" t="str">
@@ -5657,7 +5726,7 @@
         <v>Medium</v>
       </c>
       <c r="O8" s="25" t="str">
-        <f>IF(ISBLANK(I8),"",IF(J8&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
       <c r="Q8" s="10"/>
@@ -5690,7 +5759,7 @@
         <v>100</v>
       </c>
       <c r="M9" s="26" t="str">
-        <f>IF(ISBLANK(I9),"",IF(AND(D9="negative",I9&lt;0),"y",IF(AND(D9="positive",I9&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N9" s="27" t="str">
@@ -5698,7 +5767,7 @@
         <v/>
       </c>
       <c r="O9" s="27" t="str">
-        <f>IF(ISBLANK(I9),"",IF(J9&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q9" s="13"/>
@@ -5731,7 +5800,7 @@
         <v>50</v>
       </c>
       <c r="M10" s="28" t="str">
-        <f>IF(ISBLANK(I10),"",IF(AND(D10="negative",I10&lt;0),"y",IF(AND(D10="positive",I10&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N10" s="29" t="str">
@@ -5739,7 +5808,7 @@
         <v/>
       </c>
       <c r="O10" s="29" t="str">
-        <f>IF(ISBLANK(I10),"",IF(J10&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
       <c r="Q10" s="16"/>
@@ -5772,7 +5841,7 @@
         <v>50</v>
       </c>
       <c r="M11" s="28" t="str">
-        <f>IF(ISBLANK(I11),"",IF(AND(D11="negative",I11&lt;0),"y",IF(AND(D11="positive",I11&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N11" s="29" t="str">
@@ -5780,7 +5849,7 @@
         <v/>
       </c>
       <c r="O11" s="29" t="str">
-        <f>IF(ISBLANK(I11),"",IF(J11&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5810,7 +5879,7 @@
         <v>50</v>
       </c>
       <c r="M12" s="28" t="str">
-        <f>IF(ISBLANK(I12),"",IF(AND(D12="negative",I12&lt;0),"y",IF(AND(D12="positive",I12&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="N12" s="29" t="str">
@@ -5818,7 +5887,7 @@
         <v/>
       </c>
       <c r="O12" s="29" t="str">
-        <f>IF(ISBLANK(I12),"",IF(J12&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -5860,7 +5929,7 @@
         <v>0.28639856302781258</v>
       </c>
       <c r="M13" s="30" t="str">
-        <f>IF(ISBLANK(I13),"",IF(AND(D13="negative",I13&lt;0),"y",IF(AND(D13="positive",I13&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N13" s="31" t="str">
@@ -5868,7 +5937,7 @@
         <v>Small</v>
       </c>
       <c r="O13" s="31" t="str">
-        <f>IF(ISBLANK(I13),"",IF(J13&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -5910,7 +5979,7 @@
         <v>0.53917866371861423</v>
       </c>
       <c r="M14" s="30" t="str">
-        <f>IF(ISBLANK(I14),"",IF(AND(D14="negative",I14&lt;0),"y",IF(AND(D14="positive",I14&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N14" s="31" t="str">
@@ -5918,7 +5987,7 @@
         <v>None</v>
       </c>
       <c r="O14" s="31" t="str">
-        <f>IF(ISBLANK(I14),"",IF(J14&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -5960,7 +6029,7 @@
         <v>0.74949119401148678</v>
       </c>
       <c r="M15" s="30" t="str">
-        <f>IF(ISBLANK(I15),"",IF(AND(D15="negative",I15&lt;0),"y",IF(AND(D15="positive",I15&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N15" s="31" t="str">
@@ -5968,7 +6037,7 @@
         <v>None</v>
       </c>
       <c r="O15" s="31" t="str">
-        <f>IF(ISBLANK(I15),"",IF(J15&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6010,7 +6079,7 @@
         <v>0.1102840897457505</v>
       </c>
       <c r="M16" s="30" t="str">
-        <f>IF(ISBLANK(I16),"",IF(AND(D16="negative",I16&lt;0),"y",IF(AND(D16="positive",I16&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N16" s="31" t="str">
@@ -6018,7 +6087,7 @@
         <v>Small</v>
       </c>
       <c r="O16" s="31" t="str">
-        <f>IF(ISBLANK(I16),"",IF(J16&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6060,7 +6129,7 @@
         <v>0.13088138129450241</v>
       </c>
       <c r="M17" s="32" t="str">
-        <f>IF(ISBLANK(I17),"",IF(AND(D17="negative",I17&lt;0),"y",IF(AND(D17="positive",I17&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N17" s="33" t="str">
@@ -6068,7 +6137,7 @@
         <v>Small</v>
       </c>
       <c r="O17" s="33" t="str">
-        <f>IF(ISBLANK(I17),"",IF(J17&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6110,7 +6179,7 @@
         <v>7.7688076382243773E-2</v>
       </c>
       <c r="M18" s="32" t="str">
-        <f>IF(ISBLANK(I18),"",IF(AND(D18="negative",I18&lt;0),"y",IF(AND(D18="positive",I18&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N18" s="33" t="str">
@@ -6118,7 +6187,7 @@
         <v>Medium</v>
       </c>
       <c r="O18" s="33" t="str">
-        <f>IF(ISBLANK(I18),"",IF(J18&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6160,7 +6229,7 @@
         <v>0.56180767007723631</v>
       </c>
       <c r="M19" s="32" t="str">
-        <f>IF(ISBLANK(I19),"",IF(AND(D19="negative",I19&lt;0),"y",IF(AND(D19="positive",I19&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N19" s="33" t="str">
@@ -6168,7 +6237,7 @@
         <v>Small</v>
       </c>
       <c r="O19" s="33" t="str">
-        <f>IF(ISBLANK(I19),"",IF(J19&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6210,7 +6279,7 @@
         <v>0.80481821639923856</v>
       </c>
       <c r="M20" s="32" t="str">
-        <f>IF(ISBLANK(I20),"",IF(AND(D20="negative",I20&lt;0),"y",IF(AND(D20="positive",I20&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="N20" s="33" t="str">
@@ -6218,7 +6287,7 @@
         <v>None</v>
       </c>
       <c r="O20" s="33" t="str">
-        <f>IF(ISBLANK(I20),"",IF(J20&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>
@@ -6260,7 +6329,7 @@
         <v>0.77081022427378798</v>
       </c>
       <c r="M21" s="32" t="str">
-        <f>IF(ISBLANK(I21),"",IF(AND(D21="negative",I21&lt;0),"y",IF(AND(D21="positive",I21&gt;0), "y","n")))</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="N21" s="33" t="str">
@@ -6268,7 +6337,7 @@
         <v>None</v>
       </c>
       <c r="O21" s="33" t="str">
-        <f>IF(ISBLANK(I21),"",IF(J21&lt;0.05,"y","n"))</f>
+        <f t="shared" si="1"/>
         <v>n</v>
       </c>
     </row>

</xml_diff>